<commit_message>
I don't know what to do next
</commit_message>
<xml_diff>
--- a/registrations.xlsx
+++ b/registrations.xlsx
@@ -407,20 +407,20 @@
         <v>Name</v>
       </c>
       <c r="B1" t="str">
+        <v>Phone Number</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Nationality</v>
+      </c>
+      <c r="D1" t="str">
         <v>Email</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Phone Number</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Nationality</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>Er-rahmaouy Abderrahmane</v>
       </c>
-      <c r="B2" t="str">
+      <c r="D2" t="str">
         <v>abderrahmane.erra@outlook.com</v>
       </c>
     </row>
@@ -428,7 +428,7 @@
       <c r="A3" t="str">
         <v>Er-rahmaouy Abderrahmane</v>
       </c>
-      <c r="B3" t="str">
+      <c r="D3" t="str">
         <v>abderrahmane.erra@outlook.com</v>
       </c>
     </row>

</xml_diff>